<commit_message>
Create the data model, create the database context
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\IABB11\2. семестр\Infosüsteemide arendamine II veebirakendused\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homeworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{409B9376-5B2C-47B8-95E8-12ABEDD00725}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E78568DD-D7EA-4C4C-A961-FE170DF400F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
     <sheet name="Nädal 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Лист1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -66,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="37">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -174,6 +175,9 @@
   </si>
   <si>
     <t>Lugesin "globalization for jQuery Validation" kohta</t>
+  </si>
+  <si>
+    <t>Kodutöö esitamine</t>
   </si>
 </sst>
 </file>
@@ -1400,8 +1404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E639A5B4-1857-4E5D-8A42-CEA038C67138}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1831,4 +1835,314 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99507A43-E27D-4C70-B99D-4D3AB9934BA8}">
+  <dimension ref="A1:J18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" customWidth="1"/>
+    <col min="6" max="6" width="6.5546875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="43.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="41"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="42"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="44"/>
+    </row>
+    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="52"/>
+      <c r="C4" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="46">
+        <v>40953</v>
+      </c>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="47"/>
+    </row>
+    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="48"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="50"/>
+    </row>
+    <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="35"/>
+      <c r="C6" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="30">
+        <v>1</v>
+      </c>
+      <c r="B7" s="26">
+        <v>43874</v>
+      </c>
+      <c r="C7" s="27">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="D7" s="27">
+        <v>0.4548611111111111</v>
+      </c>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28">
+        <v>15</v>
+      </c>
+      <c r="G7" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="17"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="31">
+        <v>2</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="33"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="30">
+        <v>3</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="9"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="31">
+        <v>4</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="9"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="30">
+        <v>5</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="9"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="31">
+        <v>6</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="9"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="30">
+        <v>7</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="9"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="31">
+        <v>8</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="9"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="30">
+        <v>9</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="9"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="31">
+        <v>10</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="9"/>
+    </row>
+    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="30">
+        <v>11</v>
+      </c>
+      <c r="B17" s="18"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="21"/>
+    </row>
+    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="37"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="24">
+        <f>SUM(F7:F17)</f>
+        <v>15</v>
+      </c>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="23"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="A2:J3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A6:B6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Customize the Details page
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homeworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E78568DD-D7EA-4C4C-A961-FE170DF400F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{893F0AAB-C2F1-4470-8795-F874C31B41BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="38">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -178,6 +178,9 @@
   </si>
   <si>
     <t>Kodutöö esitamine</t>
+  </si>
+  <si>
+    <t>Kodutöö 3</t>
   </si>
 </sst>
 </file>
@@ -1842,7 +1845,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1948,25 +1951,25 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="30">
         <v>1</v>
       </c>
       <c r="B7" s="26">
-        <v>43874</v>
+        <v>43872</v>
       </c>
       <c r="C7" s="27">
-        <v>0.44444444444444442</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D7" s="27">
-        <v>0.4548611111111111</v>
+        <v>0.39583333333333331</v>
       </c>
       <c r="E7" s="28"/>
       <c r="F7" s="28">
-        <v>15</v>
+        <v>90</v>
       </c>
       <c r="G7" s="29" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="H7" s="25" t="s">
         <v>13</v>
@@ -1980,26 +1983,46 @@
       <c r="A8" s="31">
         <v>2</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="6"/>
+      <c r="B8" s="26">
+        <v>43874</v>
+      </c>
+      <c r="C8" s="27">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="D8" s="27">
+        <v>0.4548611111111111</v>
+      </c>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28">
+        <v>15</v>
+      </c>
+      <c r="G8" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>16</v>
+      </c>
       <c r="J8" s="33"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="30">
         <v>3</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
+      <c r="B9" s="7">
+        <v>43876</v>
+      </c>
+      <c r="C9" s="8">
+        <v>0.95833333333333337</v>
+      </c>
       <c r="D9" s="8"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
-      <c r="G9" s="6"/>
+      <c r="G9" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="H9" s="32"/>
       <c r="I9" s="6"/>
       <c r="J9" s="9"/>
@@ -2126,7 +2149,7 @@
       <c r="E18" s="38"/>
       <c r="F18" s="24">
         <f>SUM(F7:F17)</f>
-        <v>15</v>
+        <v>105</v>
       </c>
       <c r="G18" s="22"/>
       <c r="H18" s="22"/>

</xml_diff>

<commit_message>
Add a search box
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homeworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{893F0AAB-C2F1-4470-8795-F874C31B41BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209AC04B-A65D-4C4B-840C-86D60805F036}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
     <sheet name="Nädal 2" sheetId="2" r:id="rId2"/>
-    <sheet name="Лист1" sheetId="3" r:id="rId3"/>
+    <sheet name="Nädal 3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="39">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>Kodutöö 3</t>
+  </si>
+  <si>
+    <t>punktid 1 - 2, alustasin p. 3.</t>
   </si>
 </sst>
 </file>
@@ -1845,13 +1848,13 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.33203125" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.21875" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5546875" customWidth="1"/>
@@ -2017,26 +2020,40 @@
       <c r="C9" s="8">
         <v>0.95833333333333337</v>
       </c>
-      <c r="D9" s="8"/>
+      <c r="D9" s="8">
+        <v>2.9861111111111113E-2</v>
+      </c>
       <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+      <c r="F9" s="5">
+        <v>103</v>
+      </c>
       <c r="G9" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="H9" s="32"/>
+      <c r="H9" s="32" t="s">
+        <v>38</v>
+      </c>
       <c r="I9" s="6"/>
-      <c r="J9" s="9"/>
+      <c r="J9" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="31">
         <v>4</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
+      <c r="B10" s="7">
+        <v>43877</v>
+      </c>
+      <c r="C10" s="8">
+        <v>0.55208333333333337</v>
+      </c>
       <c r="D10" s="8"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="6"/>
+      <c r="G10" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
       <c r="J10" s="9"/>
@@ -2149,7 +2166,7 @@
       <c r="E18" s="38"/>
       <c r="F18" s="24">
         <f>SUM(F7:F17)</f>
-        <v>105</v>
+        <v>208</v>
       </c>
       <c r="G18" s="22"/>
       <c r="H18" s="22"/>

</xml_diff>

<commit_message>
Add a tracking property
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homeworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209AC04B-A65D-4C4B-840C-86D60805F036}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{777C1890-B03A-4C44-8537-BF6490667F05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="40">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -184,6 +184,9 @@
   </si>
   <si>
     <t>punktid 1 - 2, alustasin p. 3.</t>
+  </si>
+  <si>
+    <t>p. 3 - 7</t>
   </si>
 </sst>
 </file>
@@ -1848,7 +1851,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2048,22 +2051,36 @@
       <c r="C10" s="8">
         <v>0.55208333333333337</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
+      <c r="D10" s="8">
+        <v>0.8979166666666667</v>
+      </c>
+      <c r="E10" s="5">
+        <v>90</v>
+      </c>
+      <c r="F10" s="5">
+        <v>408</v>
+      </c>
       <c r="G10" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="6"/>
+      <c r="H10" s="6" t="s">
+        <v>39</v>
+      </c>
       <c r="I10" s="6"/>
-      <c r="J10" s="9"/>
+      <c r="J10" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="30">
         <v>5</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
+      <c r="B11" s="7">
+        <v>43877</v>
+      </c>
+      <c r="C11" s="8">
+        <v>0.98263888888888884</v>
+      </c>
       <c r="D11" s="8"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
@@ -2166,7 +2183,7 @@
       <c r="E18" s="38"/>
       <c r="F18" s="24">
         <f>SUM(F7:F17)</f>
-        <v>208</v>
+        <v>616</v>
       </c>
       <c r="G18" s="22"/>
       <c r="H18" s="22"/>

</xml_diff>

<commit_message>
Create the Person class
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homeworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{777C1890-B03A-4C44-8537-BF6490667F05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5541592-FAAA-40C4-941B-B5FBC38972AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="41">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>p. 3 - 7</t>
+  </si>
+  <si>
+    <t>p. 8</t>
   </si>
 </sst>
 </file>
@@ -1851,19 +1854,18 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.33203125" customWidth="1"/>
     <col min="2" max="2" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="5.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5546875" customWidth="1"/>
     <col min="6" max="6" width="6.5546875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="43.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.44140625" customWidth="1"/>
+    <col min="8" max="8" width="30.5546875" customWidth="1"/>
     <col min="9" max="9" width="2.109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="2.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -2081,24 +2083,40 @@
       <c r="C11" s="8">
         <v>0.98263888888888884</v>
       </c>
-      <c r="D11" s="8"/>
+      <c r="D11" s="8">
+        <v>44005.962500000001</v>
+      </c>
       <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
+      <c r="F11" s="5">
+        <v>31</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>40</v>
+      </c>
       <c r="I11" s="6"/>
-      <c r="J11" s="9"/>
+      <c r="J11" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="31">
         <v>6</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
+      <c r="B12" s="7">
+        <v>43877</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0.64027777777777783</v>
+      </c>
       <c r="D12" s="8"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
-      <c r="G12" s="6"/>
+      <c r="G12" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="9"/>
@@ -2183,7 +2201,7 @@
       <c r="E18" s="38"/>
       <c r="F18" s="24">
         <f>SUM(F7:F17)</f>
-        <v>616</v>
+        <v>647</v>
       </c>
       <c r="G18" s="22"/>
       <c r="H18" s="22"/>

</xml_diff>